<commit_message>
1. updated Default sites, Country specific and sponsor specific sites to sync with the changes made to add institute related sites 2. Review pending now includes single component matches as well
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_3.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_3.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>Project Number</t>
   </si>
@@ -70,29 +70,41 @@
     <t>Principal</t>
   </si>
   <si>
-    <t>#859015</t>
-  </si>
-  <si>
-    <t>0506/0708</t>
-  </si>
-  <si>
-    <t>Brown, Raymond Sean</t>
-  </si>
-  <si>
-    <t>Brown</t>
-  </si>
-  <si>
-    <t>Raymond</t>
-  </si>
-  <si>
-    <t>Sean</t>
+    <t>0102/0304</t>
+  </si>
+  <si>
+    <t>DeLuca Jr., William F MD</t>
+  </si>
+  <si>
+    <t>DeLuca</t>
+  </si>
+  <si>
+    <t>William</t>
+  </si>
+  <si>
+    <t>Apollo</t>
+  </si>
+  <si>
+    <t>abc street</t>
+  </si>
+  <si>
+    <t>NY</t>
+  </si>
+  <si>
+    <t>US</t>
+  </si>
+  <si>
+    <t>Spain</t>
+  </si>
+  <si>
+    <t>#6789</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -111,6 +123,18 @@
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF333333"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -150,7 +174,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -158,10 +182,19 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -466,7 +499,7 @@
   <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -562,26 +595,46 @@
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" s="5"/>
+      <c r="I2" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H2" t="s">
+      <c r="J2" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="Q2" t="s">
-        <v>18</v>
+      <c r="L2" s="4"/>
+      <c r="M2" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="N2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="O2" s="4">
+        <v>889</v>
+      </c>
+      <c r="P2" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="Q2" s="4" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Assigned to repository is ready yet to test the code
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_3.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
   <si>
     <t>Project Number</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Medical License Number</t>
   </si>
   <si>
-    <t>0102/0304</t>
-  </si>
-  <si>
     <t>William</t>
   </si>
   <si>
@@ -134,6 +131,15 @@
   </si>
   <si>
     <t>Sub I</t>
+  </si>
+  <si>
+    <t>Project Number 2</t>
+  </si>
+  <si>
+    <t>0000/0304</t>
+  </si>
+  <si>
+    <t>0102/0000</t>
   </si>
 </sst>
 </file>
@@ -542,192 +548,199 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q5"/>
+  <dimension ref="A1:R5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="19" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="23" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.28515625" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="18.5703125" customWidth="1"/>
-    <col min="24" max="24" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.28515625" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.5703125" customWidth="1"/>
+    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D2" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="I2" s="5"/>
+      <c r="J2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="4">
+        <v>889</v>
+      </c>
+      <c r="Q2" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="4" t="s">
+      <c r="E3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>38</v>
+      </c>
+      <c r="E4" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J4" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H5" t="s">
         <v>16</v>
       </c>
-      <c r="C2" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="D2" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H2" s="5"/>
-      <c r="I2" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="L2" s="4"/>
-      <c r="M2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="N2" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="O2" s="4">
-        <v>889</v>
-      </c>
-      <c r="P2" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D3" t="s">
-        <v>27</v>
-      </c>
-      <c r="G3" t="s">
-        <v>28</v>
-      </c>
-      <c r="I3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>39</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="I5" t="s">
         <v>33</v>
       </c>
-      <c r="G5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="J5" t="s">
         <v>34</v>
-      </c>
-      <c r="I5" t="s">
-        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
QC workflow has been tested and is working as expected. Created 'Completed ICSFs' page and able to display completed icsfs
</commit_message>
<xml_diff>
--- a/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_3.xlsx
+++ b/Documents/Technical/TestUpload/DDAS_Upload_CaseStudy_3.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Project Number</t>
   </si>
@@ -130,9 +130,6 @@
     <t>PI</t>
   </si>
   <si>
-    <t>Sub I</t>
-  </si>
-  <si>
     <t>Project Number 2</t>
   </si>
   <si>
@@ -140,6 +137,18 @@
   </si>
   <si>
     <t>0102/0000</t>
+  </si>
+  <si>
+    <t>Sponsor Protocol Number 2</t>
+  </si>
+  <si>
+    <t>0002/0000</t>
+  </si>
+  <si>
+    <t>0003/0000</t>
+  </si>
+  <si>
+    <t>0004/0000</t>
   </si>
 </sst>
 </file>
@@ -548,10 +557,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:R5"/>
+  <dimension ref="A1:S5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -560,41 +569,42 @@
     <col min="2" max="2" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="40.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="24.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="23" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="19.28515625" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.5703125" customWidth="1"/>
-    <col min="25" max="25" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="19.5703125" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="40.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="23" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="23" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.28515625" customWidth="1"/>
+    <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.5703125" customWidth="1"/>
+    <col min="26" max="26" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="14.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>36</v>
       </c>
@@ -602,144 +612,162 @@
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>37</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="9">
+        <v>97565</v>
+      </c>
+      <c r="F2" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="3"/>
       <c r="G2" s="3"/>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="3"/>
+      <c r="I2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I2" s="5"/>
-      <c r="J2" s="4" t="s">
+      <c r="J2" s="5"/>
+      <c r="K2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="M2" s="4"/>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="4"/>
+      <c r="O2" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="P2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="P2" s="4">
+      <c r="Q2" s="4">
         <v>889</v>
       </c>
-      <c r="Q2" s="7" t="s">
+      <c r="R2" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="4" t="s">
+      <c r="S2" s="4" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" t="s">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3" s="4"/>
+      <c r="F3" t="s">
         <v>26</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>27</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>38</v>
-      </c>
-      <c r="E4" t="s">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4" s="4"/>
+      <c r="F4" t="s">
         <v>29</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>30</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>38</v>
-      </c>
-      <c r="E5" t="s">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5" s="4"/>
+      <c r="F5" t="s">
         <v>32</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>16</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>33</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>